<commit_message>
param study changes after first xe fixes
</commit_message>
<xml_diff>
--- a/ParamStudy/findZeta.xlsx
+++ b/ParamStudy/findZeta.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="findZeta" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>CASE</t>
   </si>
@@ -33,9 +33,6 @@
     <t>TAU</t>
   </si>
   <si>
-    <t>NaN</t>
-  </si>
-  <si>
     <t>PTAU</t>
   </si>
 </sst>
@@ -43,7 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +171,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -526,9 +529,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -850,668 +854,1240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>19</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>0.110143462740471</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>6.5564901427205405E-2</v>
       </c>
-      <c r="E2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="E2" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>5.7195171241138799E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>6.6773552202674294E-2</v>
       </c>
-      <c r="E3" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="E3" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>21</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>2.1194490833978501E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>6.7968627661373293E-2</v>
       </c>
-      <c r="E4">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="E4" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>16</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>0.23084775373086</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>5.99681426227456E-2</v>
       </c>
-      <c r="E5">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="E5" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>21</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>4.1634847714850497E-3</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>6.5797153907064504E-2</v>
       </c>
-      <c r="E6">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="E6" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>22</v>
       </c>
-      <c r="E7">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="C7" s="1">
+        <v>2.5531000000000002E-4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6.6895999999999997E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
         <v>2</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>23</v>
       </c>
-      <c r="E8">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6.7949999999999997E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
         <v>2</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>25</v>
       </c>
-      <c r="E9">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6.9935999999999998E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>2</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>31</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
         <v>7.5080291363012294E-2</v>
       </c>
-      <c r="E10">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="E10" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>3</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11">
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>7.5080291363012294E-2</v>
+      </c>
+      <c r="E11" s="1">
         <v>8.2000000000000003E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>41</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
         <v>8.1839462044513894E-2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>8.2000000000000003E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
         <v>3</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>8.2427E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
         <v>43</v>
       </c>
-      <c r="E13">
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8.3002000000000006E-2</v>
+      </c>
+      <c r="E14" s="1">
         <v>8.2000000000000003E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="1">
         <v>45</v>
       </c>
-      <c r="E14">
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>8.4115999999999996E-2</v>
+      </c>
+      <c r="E15" s="1">
         <v>8.2000000000000003E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
         <v>3</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="1">
         <v>51</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
         <v>8.7200748097395295E-2</v>
       </c>
-      <c r="E15">
+      <c r="E16" s="1">
         <v>8.2000000000000003E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
         <v>10</v>
       </c>
-      <c r="B16">
+      <c r="B17" s="1">
         <v>18</v>
       </c>
-      <c r="E16">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="C17" s="1">
+        <v>0.15015999999999999</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6.6316E-2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
         <v>10</v>
       </c>
-      <c r="B17">
+      <c r="B18" s="1">
         <v>19</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>6.7643999999999996E-2</v>
-      </c>
-      <c r="E17">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="C18" s="1">
+        <v>9.1061000000000003E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6.7561999999999997E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
         <v>10</v>
       </c>
-      <c r="B18">
+      <c r="B19" s="2">
         <v>20</v>
       </c>
-      <c r="E18">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="C19" s="2">
+        <v>4.2899E-2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>6.8806000000000006E-2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
         <v>11</v>
       </c>
-      <c r="B19">
+      <c r="B20" s="1">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>8.1032000000000007E-2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>11</v>
+      </c>
+      <c r="B21" s="2">
+        <v>33</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>8.1848000000000004E-2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>11</v>
+      </c>
+      <c r="B22" s="1">
+        <v>34</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>8.2641999999999993E-2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>11</v>
+      </c>
+      <c r="B23" s="1">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>8.3412E-2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>18</v>
+      </c>
+      <c r="B24" s="2">
+        <v>53</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>6.5860000000000002E-2</v>
+      </c>
+      <c r="E24" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>18</v>
+      </c>
+      <c r="B25" s="1">
+        <v>54</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>6.6194000000000003E-2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1">
+        <v>55</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>6.6521999999999998E-2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>19</v>
+      </c>
+      <c r="B27" s="1">
+        <v>120</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>8.0531000000000005E-2</v>
+      </c>
+      <c r="E27" s="1">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>19</v>
+      </c>
+      <c r="B28" s="2">
+        <v>130</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>8.1978428089316699E-2</v>
+      </c>
+      <c r="E28" s="2">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1">
+        <v>131</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>8.2116999999999996E-2</v>
+      </c>
+      <c r="E29" s="1">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>19</v>
+      </c>
+      <c r="B30" s="1">
+        <v>140</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>8.3320000000000005E-2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>26</v>
+      </c>
+      <c r="B31" s="2">
+        <v>53</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>6.5860000000000002E-2</v>
+      </c>
+      <c r="E31" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>26</v>
+      </c>
+      <c r="B32" s="1">
+        <v>54</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>6.6194000000000003E-2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>27</v>
+      </c>
+      <c r="B33" s="1">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>8.0531000000000005E-2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>27</v>
+      </c>
+      <c r="B34" s="2">
+        <v>130</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>8.1977999999999995E-2</v>
+      </c>
+      <c r="E34" s="2">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>27</v>
+      </c>
+      <c r="B35" s="1">
+        <v>140</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <v>8.3320000000000005E-2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1">
+        <v>15</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.21844</v>
+      </c>
+      <c r="D36" s="1">
+        <v>8.0836000000000005E-2</v>
+      </c>
+      <c r="E36" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>34</v>
+      </c>
+      <c r="B37" s="1">
+        <v>22</v>
+      </c>
+      <c r="C37" s="1">
+        <v>7.6855000000000007E-2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>9.0879000000000001E-2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>34</v>
+      </c>
+      <c r="B38" s="1">
+        <v>23</v>
+      </c>
+      <c r="C38" s="1">
+        <v>6.0031000000000001E-2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>9.2121999999999996E-2</v>
+      </c>
+      <c r="E38" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>34</v>
+      </c>
+      <c r="B39" s="2">
+        <v>24</v>
+      </c>
+      <c r="C39" s="2">
+        <v>4.5373999999999998E-2</v>
+      </c>
+      <c r="D39" s="2">
+        <v>9.3325000000000005E-2</v>
+      </c>
+      <c r="E39" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>34</v>
+      </c>
+      <c r="B40" s="1">
+        <v>25</v>
+      </c>
+      <c r="C40" s="1">
+        <v>3.2960000000000003E-2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>9.4488000000000003E-2</v>
+      </c>
+      <c r="E40" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>35</v>
+      </c>
+      <c r="B41" s="1">
+        <v>20</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.11532000000000001</v>
+      </c>
+      <c r="D41" s="1">
+        <v>8.8265999999999997E-2</v>
+      </c>
+      <c r="E41" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>35</v>
+      </c>
+      <c r="B42" s="2">
+        <v>28</v>
+      </c>
+      <c r="C42" s="2">
+        <v>9.8239E-3</v>
+      </c>
+      <c r="D42" s="2">
+        <v>9.7753999999999994E-2</v>
+      </c>
+      <c r="E42" s="2">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
+        <v>35</v>
+      </c>
+      <c r="B43" s="1">
+        <v>29</v>
+      </c>
+      <c r="C43" s="1">
+        <v>6.3763999999999999E-3</v>
+      </c>
+      <c r="D43" s="1">
+        <v>9.8770999999999998E-2</v>
+      </c>
+      <c r="E43" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>35</v>
+      </c>
+      <c r="B44" s="1">
         <v>30</v>
       </c>
-      <c r="E19">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>11</v>
-      </c>
-      <c r="B20">
-        <v>32</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>8.1032000000000007E-2</v>
-      </c>
-      <c r="E20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>11</v>
-      </c>
-      <c r="B21">
+      <c r="C44" s="1">
+        <v>3.5565000000000002E-3</v>
+      </c>
+      <c r="D44" s="1">
+        <v>9.9755999999999997E-2</v>
+      </c>
+      <c r="E44" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
         <v>35</v>
       </c>
-      <c r="E21">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>18</v>
-      </c>
-      <c r="B22">
-        <v>53</v>
-      </c>
-      <c r="E22">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>18</v>
-      </c>
-      <c r="B23">
-        <v>54</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>6.6194000000000003E-2</v>
-      </c>
-      <c r="E23">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>18</v>
-      </c>
-      <c r="B24">
-        <v>55</v>
-      </c>
-      <c r="E24">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>19</v>
-      </c>
-      <c r="B25">
-        <v>120</v>
-      </c>
-      <c r="E25">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>19</v>
-      </c>
-      <c r="B26">
-        <v>130</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>8.1978428089316699E-2</v>
-      </c>
-      <c r="E26">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>19</v>
-      </c>
-      <c r="B27">
-        <v>140</v>
-      </c>
-      <c r="E27">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>53</v>
-      </c>
-      <c r="E28">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>26</v>
-      </c>
-      <c r="B29">
-        <v>54</v>
-      </c>
-      <c r="E29">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>26</v>
-      </c>
-      <c r="B30">
-        <v>55</v>
-      </c>
-      <c r="E30">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>27</v>
-      </c>
-      <c r="B31">
-        <v>120</v>
-      </c>
-      <c r="E31">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>27</v>
-      </c>
-      <c r="B32">
-        <v>130</v>
-      </c>
-      <c r="E32">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>27</v>
-      </c>
-      <c r="B33">
-        <v>140</v>
-      </c>
-      <c r="E33">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>34</v>
-      </c>
-      <c r="B34">
-        <v>15</v>
-      </c>
-      <c r="E34">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
+      <c r="B45" s="1">
+        <v>40</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.10813</v>
+      </c>
+      <c r="E45" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>42</v>
+      </c>
+      <c r="B46" s="1">
+        <v>20</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.11532000000000001</v>
+      </c>
+      <c r="D46" s="1">
+        <v>8.8265999999999997E-2</v>
+      </c>
+      <c r="E46" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>42</v>
+      </c>
+      <c r="B47" s="1">
         <v>25</v>
       </c>
-      <c r="E35">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>20</v>
-      </c>
-      <c r="E36">
+      <c r="C47" s="1">
+        <v>3.2960000000000003E-2</v>
+      </c>
+      <c r="D47" s="1">
+        <v>9.4488000000000003E-2</v>
+      </c>
+      <c r="E47" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>43</v>
+      </c>
+      <c r="B48" s="2">
+        <v>28</v>
+      </c>
+      <c r="C48" s="2">
+        <v>9.8239E-3</v>
+      </c>
+      <c r="D48" s="2">
+        <v>9.7753999999999994E-2</v>
+      </c>
+      <c r="E48" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>35</v>
-      </c>
-      <c r="B37">
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>43</v>
+      </c>
+      <c r="B49" s="1">
         <v>30</v>
       </c>
-      <c r="E37">
+      <c r="C49" s="1">
+        <v>3.5565000000000002E-3</v>
+      </c>
+      <c r="D49" s="1">
+        <v>9.9755999999999997E-2</v>
+      </c>
+      <c r="E49" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>35</v>
-      </c>
-      <c r="B38">
-        <v>40</v>
-      </c>
-      <c r="E38">
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>50</v>
+      </c>
+      <c r="B50" s="1">
+        <v>400</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>6.4458000000000001E-2</v>
+      </c>
+      <c r="E50" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1">
+        <v>450</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1">
+        <v>6.5874000000000002E-2</v>
+      </c>
+      <c r="E51" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" s="1">
+        <v>454</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1">
+        <v>6.5980999999999998E-2</v>
+      </c>
+      <c r="E52" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="2">
+        <v>50</v>
+      </c>
+      <c r="B53" s="2">
+        <v>455</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0</v>
+      </c>
+      <c r="D53" s="2">
+        <v>6.6006999999999996E-2</v>
+      </c>
+      <c r="E53" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>50</v>
+      </c>
+      <c r="B54" s="1">
+        <v>460</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1">
+        <v>6.6140000000000004E-2</v>
+      </c>
+      <c r="E54" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
+        <v>50</v>
+      </c>
+      <c r="B55" s="1">
+        <v>465</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1">
+        <v>6.6269999999999996E-2</v>
+      </c>
+      <c r="E55" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>51</v>
+      </c>
+      <c r="B56" s="1">
+        <v>800</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1">
+        <v>7.2978000000000001E-2</v>
+      </c>
+      <c r="E56" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>42</v>
-      </c>
-      <c r="B39">
-        <v>15</v>
-      </c>
-      <c r="E39">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>42</v>
-      </c>
-      <c r="B40">
-        <v>25</v>
-      </c>
-      <c r="E40">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <v>43</v>
-      </c>
-      <c r="B41">
-        <v>20</v>
-      </c>
-      <c r="E41">
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>51</v>
+      </c>
+      <c r="B57" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1">
+        <v>8.9252999999999999E-2</v>
+      </c>
+      <c r="E57" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <v>43</v>
-      </c>
-      <c r="B42">
-        <v>30</v>
-      </c>
-      <c r="E42">
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>51</v>
+      </c>
+      <c r="B58" s="1">
+        <v>6000</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1">
+        <v>9.7882999999999998E-2</v>
+      </c>
+      <c r="E58" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>43</v>
-      </c>
-      <c r="B43">
-        <v>40</v>
-      </c>
-      <c r="E43">
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>51</v>
+      </c>
+      <c r="B59" s="1">
+        <v>6050</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1">
+        <v>9.7987000000000005E-2</v>
+      </c>
+      <c r="E59" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <v>50</v>
-      </c>
-      <c r="E44">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>50</v>
-      </c>
-      <c r="E45">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <v>50</v>
-      </c>
-      <c r="E46">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47">
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="2">
         <v>51</v>
       </c>
-      <c r="E47">
+      <c r="B60" s="2">
+        <v>6060</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2">
+        <v>9.8006999999999997E-2</v>
+      </c>
+      <c r="E60" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48">
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
         <v>51</v>
       </c>
-      <c r="E48">
+      <c r="B61" s="1">
+        <v>6080</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1">
+        <v>9.8047999999999996E-2</v>
+      </c>
+      <c r="E61" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49">
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
         <v>51</v>
       </c>
-      <c r="E49">
+      <c r="B62" s="1">
+        <v>6100</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1">
+        <v>9.8088999999999996E-2</v>
+      </c>
+      <c r="E62" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50">
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>51</v>
+      </c>
+      <c r="B63" s="1">
+        <v>6120</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1">
+        <v>9.8129999999999995E-2</v>
+      </c>
+      <c r="E63" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>51</v>
+      </c>
+      <c r="B64" s="1">
+        <v>6200</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1">
+        <v>9.8291000000000003E-2</v>
+      </c>
+      <c r="E64" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
         <v>58</v>
       </c>
-      <c r="E50">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51">
+      <c r="B65" s="1">
+        <v>400</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1">
+        <v>6.4458000000000001E-2</v>
+      </c>
+      <c r="E65" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
         <v>58</v>
       </c>
-      <c r="E51">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>58</v>
-      </c>
-      <c r="E52">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53">
+      <c r="B66" s="1">
+        <v>450</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1">
+        <v>6.5874000000000002E-2</v>
+      </c>
+      <c r="E66" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" s="1">
         <v>59</v>
       </c>
-      <c r="E53">
+      <c r="B67" s="1">
+        <v>6000</v>
+      </c>
+      <c r="C67" s="1">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1">
+        <v>9.7882999999999998E-2</v>
+      </c>
+      <c r="E67" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54">
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
         <v>59</v>
       </c>
-      <c r="E54">
+      <c r="B68" s="1">
+        <v>6200</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1">
+        <v>9.8291000000000003E-2</v>
+      </c>
+      <c r="E68" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55">
-        <v>59</v>
-      </c>
-      <c r="E55">
-        <v>9.8000000000000004E-2</v>
-      </c>
+      <c r="F68" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
param study general work
</commit_message>
<xml_diff>
--- a/ParamStudy/findZeta.xlsx
+++ b/ParamStudy/findZeta.xlsx
@@ -854,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2086,6 +2086,270 @@
       </c>
       <c r="F68" s="1"/>
     </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>66</v>
+      </c>
+      <c r="B69" s="1">
+        <v>16</v>
+      </c>
+      <c r="E69" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>66</v>
+      </c>
+      <c r="B70" s="1">
+        <v>18</v>
+      </c>
+      <c r="E70" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>66</v>
+      </c>
+      <c r="B71" s="1">
+        <v>20</v>
+      </c>
+      <c r="E71" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>67</v>
+      </c>
+      <c r="B72" s="1">
+        <v>18</v>
+      </c>
+      <c r="E72" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>67</v>
+      </c>
+      <c r="B73" s="1">
+        <v>19</v>
+      </c>
+      <c r="E73" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>67</v>
+      </c>
+      <c r="B74" s="1">
+        <v>20</v>
+      </c>
+      <c r="E74" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>68</v>
+      </c>
+      <c r="B75" s="1">
+        <v>20</v>
+      </c>
+      <c r="E75" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>68</v>
+      </c>
+      <c r="B76" s="1">
+        <v>21</v>
+      </c>
+      <c r="E76" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>68</v>
+      </c>
+      <c r="B77" s="1">
+        <v>22</v>
+      </c>
+      <c r="E77" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>69</v>
+      </c>
+      <c r="B78" s="1">
+        <v>20</v>
+      </c>
+      <c r="E78" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>69</v>
+      </c>
+      <c r="B79" s="1">
+        <v>25</v>
+      </c>
+      <c r="E79" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>69</v>
+      </c>
+      <c r="B80" s="1">
+        <v>30</v>
+      </c>
+      <c r="E80" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>70</v>
+      </c>
+      <c r="B81" s="1">
+        <v>16</v>
+      </c>
+      <c r="E81" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>70</v>
+      </c>
+      <c r="B82" s="1">
+        <v>18</v>
+      </c>
+      <c r="E82" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>70</v>
+      </c>
+      <c r="B83" s="1">
+        <v>20</v>
+      </c>
+      <c r="E83" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>71</v>
+      </c>
+      <c r="B84" s="1">
+        <v>20</v>
+      </c>
+      <c r="E84" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>71</v>
+      </c>
+      <c r="B85" s="1">
+        <v>30</v>
+      </c>
+      <c r="E85" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>71</v>
+      </c>
+      <c r="B86" s="1">
+        <v>50</v>
+      </c>
+      <c r="E86" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>72</v>
+      </c>
+      <c r="B87" s="1">
+        <v>20</v>
+      </c>
+      <c r="E87" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>72</v>
+      </c>
+      <c r="B88" s="1">
+        <v>50</v>
+      </c>
+      <c r="E88" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>72</v>
+      </c>
+      <c r="B89" s="1">
+        <v>100</v>
+      </c>
+      <c r="E89" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>73</v>
+      </c>
+      <c r="B90" s="1">
+        <v>20</v>
+      </c>
+      <c r="E90" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>73</v>
+      </c>
+      <c r="B91" s="1">
+        <v>200</v>
+      </c>
+      <c r="E91" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>73</v>
+      </c>
+      <c r="B92" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E92" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Some stuff so Aviad can checkout
</commit_message>
<xml_diff>
--- a/ParamStudy/findZeta.xlsx
+++ b/ParamStudy/findZeta.xlsx
@@ -15,7 +15,7 @@
     <sheet name="findZeta" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">findZeta!$A$1:$F$207</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">findZeta!$A$1:$F$208</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -882,15 +882,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F207"/>
+  <dimension ref="A1:F218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="C205" sqref="C205"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" style="12"/>
     <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
@@ -936,7 +936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -973,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>5</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>6</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>7</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>8</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>8</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>9</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>9</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>9</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>10</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>10</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>11</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>11</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>11</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>12</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>12</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>13</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>13</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>14</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>15</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>15</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>15</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>16</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>17</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>17</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="14">
         <v>17</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>18</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>18</v>
       </c>
@@ -1838,7 +1838,7 @@
       </c>
       <c r="F52" s="17"/>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>18</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>19</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>19</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>19</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>19</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>19</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>20</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>20</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>20</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>20</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>20</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>21</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>21</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>21</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>21</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>21</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>22</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>22</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>22</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>23</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>23</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>24</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>24</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>25</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>25</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>26</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>26</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>27</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>27</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>28</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>28</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>29</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>29</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>30</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>30</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>31</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>31</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>32</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>32</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>33</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>33</v>
       </c>
@@ -2835,196 +2835,196 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>34</v>
       </c>
       <c r="B109" s="1">
-        <v>0.1</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="C109">
         <v>0</v>
       </c>
       <c r="D109" s="12">
-        <v>0.11139</v>
+        <v>0.11117</v>
       </c>
       <c r="E109" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>34</v>
       </c>
       <c r="B110" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C110">
         <v>0</v>
       </c>
       <c r="D110" s="12">
-        <v>0.11212999999999999</v>
+        <v>0.11139</v>
       </c>
       <c r="E110" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>34</v>
       </c>
       <c r="B111" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C111">
         <v>0</v>
       </c>
       <c r="D111" s="12">
-        <v>0.113023074392321</v>
+        <v>0.11212999999999999</v>
       </c>
       <c r="E111" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>34</v>
       </c>
       <c r="B112" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C112">
         <v>0</v>
       </c>
       <c r="D112" s="12">
-        <v>0.114650366905687</v>
+        <v>0.113023074392321</v>
       </c>
       <c r="E112" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>34</v>
       </c>
       <c r="B113" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C113">
         <v>0</v>
       </c>
       <c r="D113" s="12">
-        <v>0.116118821094439</v>
+        <v>0.114650366905687</v>
       </c>
       <c r="E113" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>34</v>
       </c>
       <c r="B114" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C114">
         <v>0</v>
       </c>
       <c r="D114" s="12">
-        <v>0.118689942564285</v>
+        <v>0.116118821094439</v>
       </c>
       <c r="E114" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>34</v>
       </c>
       <c r="B115" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C115">
         <v>0</v>
       </c>
       <c r="D115" s="12">
-        <v>0.12379011650249699</v>
+        <v>0.118689942564285</v>
       </c>
       <c r="E115" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>34</v>
       </c>
       <c r="B116" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C116">
         <v>0</v>
       </c>
       <c r="D116" s="12">
-        <v>0.127764655693102</v>
+        <v>0.12379011650249699</v>
       </c>
       <c r="E116" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>34</v>
       </c>
       <c r="B117" s="1">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C117">
         <v>0</v>
       </c>
       <c r="D117" s="12">
-        <v>0.13217772709937101</v>
+        <v>0.127764655693102</v>
       </c>
       <c r="E117" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>34</v>
       </c>
       <c r="B118" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C118">
         <v>0</v>
       </c>
       <c r="D118" s="12">
-        <v>0.133268036681116</v>
+        <v>0.13217772709937101</v>
       </c>
       <c r="E118" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>34</v>
       </c>
       <c r="B119" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C119">
         <v>0</v>
       </c>
       <c r="D119" s="12">
-        <v>0.13429889487799501</v>
+        <v>0.133268036681116</v>
       </c>
       <c r="E119" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B120" s="1">
         <v>26</v>
@@ -3036,368 +3036,368 @@
         <v>0.13429889487799501</v>
       </c>
       <c r="E120" s="1">
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>35</v>
       </c>
-      <c r="B121">
-        <v>28</v>
+      <c r="B121" s="1">
+        <v>26</v>
       </c>
       <c r="C121">
         <v>0</v>
       </c>
       <c r="D121" s="12">
-        <v>0.13527628359232799</v>
+        <v>0.13429889487799501</v>
       </c>
       <c r="E121" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>35</v>
       </c>
-      <c r="B122" s="1">
-        <v>30</v>
+      <c r="B122">
+        <v>28</v>
       </c>
       <c r="C122">
         <v>0</v>
       </c>
       <c r="D122" s="12">
-        <v>0.13620479631384699</v>
+        <v>0.13527628359232799</v>
       </c>
       <c r="E122" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123">
+        <v>35</v>
+      </c>
+      <c r="B123" s="1">
+        <v>30</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123" s="12">
+        <v>0.13620479631384699</v>
+      </c>
+      <c r="E123" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A124">
         <v>36</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B124" s="1">
         <v>20</v>
       </c>
-      <c r="C123">
+      <c r="C124">
         <v>6.7501982119299697E-2</v>
       </c>
-      <c r="D123" s="12">
+      <c r="D124" s="12">
         <v>8.9400581692057404E-2</v>
       </c>
-      <c r="E123" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A124" s="3">
+      <c r="E124" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A125" s="3">
         <v>36</v>
       </c>
-      <c r="B124" s="2">
+      <c r="B125" s="2">
         <v>21</v>
       </c>
-      <c r="C124" s="3">
+      <c r="C125" s="3">
         <v>5.0975006846763801E-2</v>
       </c>
-      <c r="D124" s="11">
+      <c r="D125" s="11">
         <v>9.0713842039298206E-2</v>
       </c>
-      <c r="E124" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F124" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A125">
-        <v>36</v>
-      </c>
-      <c r="B125" s="1">
-        <v>22</v>
-      </c>
-      <c r="C125">
-        <v>3.9790006381624603E-2</v>
-      </c>
-      <c r="D125" s="12">
-        <v>9.1978394456073698E-2</v>
-      </c>
-      <c r="E125" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="E125" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F125" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>36</v>
       </c>
       <c r="B126" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C126">
-        <v>2.01326070242057E-2</v>
+        <v>3.9790006381624603E-2</v>
       </c>
       <c r="D126" s="12">
-        <v>9.4376312009583796E-2</v>
+        <v>9.1978394456073698E-2</v>
       </c>
       <c r="E126" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>36</v>
       </c>
       <c r="B127" s="1">
+        <v>24</v>
+      </c>
+      <c r="C127">
+        <v>2.01326070242057E-2</v>
+      </c>
+      <c r="D127" s="12">
+        <v>9.4376312009583796E-2</v>
+      </c>
+      <c r="E127" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>36</v>
+      </c>
+      <c r="B128" s="1">
         <v>26</v>
       </c>
-      <c r="C127">
+      <c r="C128">
         <v>8.7349938877987095E-3</v>
       </c>
-      <c r="D127" s="12">
+      <c r="D128" s="12">
         <v>9.6608014506346304E-2</v>
       </c>
-      <c r="E127" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A128" s="3">
+      <c r="E128" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A129" s="3">
         <v>37</v>
       </c>
-      <c r="B128" s="2">
+      <c r="B129" s="2">
         <v>27</v>
       </c>
-      <c r="C128" s="3">
+      <c r="C129" s="3">
         <v>5.8956161712017301E-3</v>
       </c>
-      <c r="D128" s="11">
+      <c r="D129" s="11">
         <v>9.7666281240496394E-2</v>
       </c>
-      <c r="E128" s="2">
+      <c r="E129" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F128" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A129">
-        <v>37</v>
-      </c>
-      <c r="B129">
-        <v>28</v>
-      </c>
-      <c r="C129">
-        <v>2.9779082810790598E-3</v>
-      </c>
-      <c r="D129" s="12">
-        <v>9.8688066464592397E-2</v>
-      </c>
-      <c r="E129" s="1">
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F129" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>37</v>
       </c>
-      <c r="B130" s="1">
-        <v>30</v>
+      <c r="B130">
+        <v>28</v>
       </c>
       <c r="C130">
-        <v>9.2652621150275899E-4</v>
+        <v>2.9779082810790598E-3</v>
       </c>
       <c r="D130" s="12">
-        <v>0.100632668824402</v>
+        <v>9.8688066464592397E-2</v>
       </c>
       <c r="E130" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A131" s="3">
+      <c r="A131">
+        <v>37</v>
+      </c>
+      <c r="B131" s="1">
+        <v>30</v>
+      </c>
+      <c r="C131">
+        <v>9.2652621150275899E-4</v>
+      </c>
+      <c r="D131" s="12">
+        <v>0.100632668824402</v>
+      </c>
+      <c r="E131" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A132" s="3">
         <v>38</v>
       </c>
-      <c r="B131" s="2">
+      <c r="B132" s="2">
         <v>22</v>
       </c>
-      <c r="C131" s="3">
+      <c r="C132" s="3">
         <v>4.4874672014504201E-2</v>
       </c>
-      <c r="D131" s="11">
+      <c r="D132" s="11">
         <v>9.2968279681362703E-2</v>
       </c>
-      <c r="E131" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F131" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A132">
+      <c r="E132" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F132" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A133">
         <v>38</v>
       </c>
-      <c r="B132" s="1">
+      <c r="B133" s="1">
         <v>24</v>
       </c>
-      <c r="C132">
+      <c r="C133">
         <v>2.2750232708473199E-2</v>
       </c>
-      <c r="D132" s="12">
+      <c r="D133" s="12">
         <v>9.5345880930685398E-2</v>
       </c>
-      <c r="E132" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="6">
+      <c r="E133" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A134" s="6">
         <v>38</v>
       </c>
-      <c r="B133" s="5">
+      <c r="B134" s="5">
         <v>26</v>
       </c>
-      <c r="C133" s="6">
+      <c r="C134" s="6">
         <v>1.03819569359855E-2</v>
       </c>
-      <c r="D133" s="13">
+      <c r="D134" s="13">
         <v>9.7559183649105194E-2</v>
       </c>
-      <c r="E133" s="5">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F133" s="6"/>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A134" s="3">
+      <c r="E134" s="5">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F134" s="6"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A135" s="3">
         <v>39</v>
       </c>
-      <c r="B134" s="2">
+      <c r="B135" s="2">
         <v>26</v>
       </c>
-      <c r="C134" s="3">
+      <c r="C135" s="3">
         <v>1.03819569359855E-2</v>
       </c>
-      <c r="D134" s="11">
+      <c r="D135" s="11">
         <v>9.7559183649105194E-2</v>
       </c>
-      <c r="E134" s="2">
+      <c r="E135" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F134" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A135">
-        <v>39</v>
-      </c>
-      <c r="B135" s="1">
-        <v>27</v>
-      </c>
-      <c r="C135">
-        <v>6.8684606463006804E-3</v>
-      </c>
-      <c r="D135" s="12">
-        <v>9.86088877517972E-2</v>
-      </c>
-      <c r="E135" s="1">
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F135" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>39</v>
       </c>
-      <c r="B136">
-        <v>28</v>
+      <c r="B136" s="1">
+        <v>27</v>
       </c>
       <c r="C136">
-        <v>3.82181506699002E-3</v>
+        <v>6.8684606463006804E-3</v>
       </c>
       <c r="D136" s="12">
-        <v>9.9622660576497907E-2</v>
+        <v>9.86088877517972E-2</v>
       </c>
       <c r="E136" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>39</v>
       </c>
-      <c r="B137" s="1">
-        <v>30</v>
+      <c r="B137">
+        <v>28</v>
       </c>
       <c r="C137">
-        <v>1.3228005154433599E-3</v>
+        <v>3.82181506699002E-3</v>
       </c>
       <c r="D137" s="12">
-        <v>0.10155172841512999</v>
+        <v>9.9622660576497907E-2</v>
       </c>
       <c r="E137" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138">
+        <v>39</v>
+      </c>
+      <c r="B138" s="1">
+        <v>30</v>
+      </c>
+      <c r="C138">
+        <v>1.3228005154433599E-3</v>
+      </c>
+      <c r="D138" s="12">
+        <v>0.10155172841512999</v>
+      </c>
+      <c r="E138" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A139">
         <v>40</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B139" s="1">
         <v>22</v>
       </c>
-      <c r="C138">
+      <c r="C139">
         <v>7.6224063203815598E-2</v>
       </c>
-      <c r="D138" s="12">
+      <c r="D139" s="12">
         <v>9.0905259439019406E-2</v>
       </c>
-      <c r="E138" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A139" s="3">
+      <c r="E139" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140" s="3">
         <v>40</v>
       </c>
-      <c r="B139" s="2">
+      <c r="B140" s="2">
         <v>24</v>
       </c>
-      <c r="C139" s="3">
+      <c r="C140" s="3">
         <v>4.4715112707687001E-2</v>
       </c>
-      <c r="D139" s="11">
+      <c r="D140" s="11">
         <v>9.3350490121472604E-2</v>
       </c>
-      <c r="E139" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F139" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A140">
+      <c r="E140" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F140" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A141">
         <v>40</v>
-      </c>
-      <c r="B140" s="1">
-        <v>26</v>
-      </c>
-      <c r="C140">
-        <v>2.4190565368510799E-2</v>
-      </c>
-      <c r="D140" s="12">
-        <v>9.5637481390108803E-2</v>
-      </c>
-      <c r="E140" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A141">
-        <v>41</v>
       </c>
       <c r="B141" s="1">
         <v>26</v>
@@ -3409,1214 +3409,1335 @@
         <v>9.5637481390108803E-2</v>
       </c>
       <c r="E141" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>41</v>
+      </c>
+      <c r="B142" s="1">
+        <v>26</v>
+      </c>
+      <c r="C142">
+        <v>2.4190565368510799E-2</v>
+      </c>
+      <c r="D142" s="12">
+        <v>9.5637481390108803E-2</v>
+      </c>
+      <c r="E142" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A142" s="3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A143" s="3">
         <v>41</v>
       </c>
-      <c r="B142" s="3">
+      <c r="B143" s="3">
         <v>28</v>
       </c>
-      <c r="C142" s="3">
+      <c r="C143" s="3">
         <v>9.5776739104209106E-3</v>
       </c>
-      <c r="D142" s="11">
+      <c r="D143" s="11">
         <v>9.7777665943820202E-2</v>
       </c>
-      <c r="E142" s="2">
+      <c r="E143" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F142" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A143">
-        <v>41</v>
-      </c>
-      <c r="B143" s="1">
-        <v>29</v>
-      </c>
-      <c r="C143">
-        <v>6.2715054542467202E-3</v>
-      </c>
-      <c r="D143" s="12">
-        <v>9.8794794817689394E-2</v>
-      </c>
-      <c r="E143" s="1">
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F143" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>41</v>
       </c>
       <c r="B144" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C144">
-        <v>3.7702483227169299E-3</v>
+        <v>6.2715054542467202E-3</v>
       </c>
       <c r="D144" s="12">
-        <v>9.9779187857661003E-2</v>
+        <v>9.8794794817689394E-2</v>
       </c>
       <c r="E144" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A145" s="3">
+      <c r="A145">
+        <v>41</v>
+      </c>
+      <c r="B145" s="1">
+        <v>30</v>
+      </c>
+      <c r="C145">
+        <v>3.7702483227169299E-3</v>
+      </c>
+      <c r="D145" s="12">
+        <v>9.9779187857661003E-2</v>
+      </c>
+      <c r="E145" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A146" s="3">
         <v>42</v>
       </c>
-      <c r="B145" s="2">
+      <c r="B146" s="2">
         <v>22</v>
       </c>
-      <c r="C145" s="3">
+      <c r="C146" s="3">
         <v>4.4874672014572202E-2</v>
       </c>
-      <c r="D145" s="11">
+      <c r="D146" s="11">
         <v>9.2968279681360705E-2</v>
       </c>
-      <c r="E145" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F145" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A146">
+      <c r="E146" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F146" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A147">
         <v>42</v>
       </c>
-      <c r="B146" s="1">
+      <c r="B147" s="1">
         <v>24</v>
       </c>
-      <c r="C146">
+      <c r="C147">
         <v>2.27502327084728E-2</v>
       </c>
-      <c r="D146" s="12">
+      <c r="D147" s="12">
         <v>9.5345880930685606E-2</v>
       </c>
-      <c r="E146" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A147" s="3">
+      <c r="E147" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A148" s="3">
         <v>43</v>
       </c>
-      <c r="B147" s="2">
+      <c r="B148" s="2">
         <v>26</v>
       </c>
-      <c r="C147" s="3">
+      <c r="C148" s="3">
         <v>1.03819569359857E-2</v>
       </c>
-      <c r="D147" s="11">
+      <c r="D148" s="11">
         <v>9.7559183649105097E-2</v>
       </c>
-      <c r="E147" s="2">
+      <c r="E148" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F147" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A148">
-        <v>43</v>
-      </c>
-      <c r="B148">
-        <v>28</v>
-      </c>
-      <c r="C148">
-        <v>3.8218150670092902E-3</v>
-      </c>
-      <c r="D148" s="12">
-        <v>9.9622660576491398E-2</v>
-      </c>
-      <c r="E148" s="1">
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F148" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>43</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149">
+        <v>28</v>
+      </c>
+      <c r="C149">
+        <v>3.8218150670092902E-3</v>
+      </c>
+      <c r="D149" s="12">
+        <v>9.9622660576491398E-2</v>
+      </c>
+      <c r="E149" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>43</v>
+      </c>
+      <c r="B150" s="1">
         <v>30</v>
       </c>
-      <c r="C149">
+      <c r="C150">
         <v>1.3228005154433901E-3</v>
       </c>
-      <c r="D149" s="12">
+      <c r="D150" s="12">
         <v>0.10155172841512999</v>
       </c>
-      <c r="E149" s="1">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A150" s="3">
+      <c r="E150" s="1">
+        <v>8.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A151" s="3">
         <v>44</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B151" s="2">
         <v>21</v>
       </c>
-      <c r="C150" s="3">
+      <c r="C151" s="3">
         <v>5.0975006846762601E-2</v>
       </c>
-      <c r="D150" s="11">
+      <c r="D151" s="11">
         <v>9.0713842039298206E-2</v>
       </c>
-      <c r="E150" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F150" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A151">
-        <v>44</v>
-      </c>
-      <c r="B151" s="1">
-        <v>22</v>
-      </c>
-      <c r="C151">
-        <v>3.9790006381619399E-2</v>
-      </c>
-      <c r="D151" s="12">
-        <v>9.1978394456073906E-2</v>
-      </c>
-      <c r="E151" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="E151" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F151" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>44</v>
       </c>
       <c r="B152" s="1">
+        <v>22</v>
+      </c>
+      <c r="C152">
+        <v>3.9790006381619399E-2</v>
+      </c>
+      <c r="D152" s="12">
+        <v>9.1978394456073906E-2</v>
+      </c>
+      <c r="E152" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>44</v>
+      </c>
+      <c r="B153" s="1">
         <v>24</v>
       </c>
-      <c r="C152">
+      <c r="C153">
         <v>2.0132607024204399E-2</v>
       </c>
-      <c r="D152" s="12">
+      <c r="D153" s="12">
         <v>9.4376312009583893E-2</v>
       </c>
-      <c r="E152" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A153">
+      <c r="E153" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A154">
         <v>45</v>
       </c>
-      <c r="B153" s="1">
+      <c r="B154" s="1">
         <v>26</v>
       </c>
-      <c r="C153">
+      <c r="C154">
         <v>8.7349938878929795E-3</v>
       </c>
-      <c r="D153" s="12">
+      <c r="D154" s="12">
         <v>9.6608014506340406E-2</v>
       </c>
-      <c r="E153" s="1">
+      <c r="E154" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A154" s="3">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A155" s="3">
         <v>45</v>
       </c>
-      <c r="B154" s="2">
+      <c r="B155" s="2">
         <v>27</v>
       </c>
-      <c r="C154" s="3">
+      <c r="C155" s="3">
         <v>5.8956161712018298E-3</v>
       </c>
-      <c r="D154" s="11">
+      <c r="D155" s="11">
         <v>9.7666281240496297E-2</v>
       </c>
-      <c r="E154" s="2">
+      <c r="E155" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F154" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A155">
-        <v>45</v>
-      </c>
-      <c r="B155">
-        <v>28</v>
-      </c>
-      <c r="C155">
-        <v>2.9779124672901498E-3</v>
-      </c>
-      <c r="D155" s="12">
-        <v>9.8688072647361E-2</v>
-      </c>
-      <c r="E155" s="1">
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F155" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>45</v>
       </c>
-      <c r="B156" s="1">
-        <v>30</v>
+      <c r="B156">
+        <v>28</v>
       </c>
       <c r="C156">
-        <v>9.2652621150281201E-4</v>
+        <v>2.9779124672901498E-3</v>
       </c>
       <c r="D156" s="12">
-        <v>0.100632668824402</v>
+        <v>9.8688072647361E-2</v>
       </c>
       <c r="E156" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157">
+        <v>45</v>
+      </c>
+      <c r="B157" s="1">
+        <v>30</v>
+      </c>
+      <c r="C157">
+        <v>9.2652621150281201E-4</v>
+      </c>
+      <c r="D157" s="12">
+        <v>0.100632668824402</v>
+      </c>
+      <c r="E157" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A158">
         <v>46</v>
       </c>
-      <c r="B157" s="1">
+      <c r="B158" s="1">
         <v>22</v>
       </c>
-      <c r="C157">
+      <c r="C158">
         <v>7.6210634131750596E-2</v>
       </c>
-      <c r="D157" s="12">
+      <c r="D158" s="12">
         <v>9.0919008549390196E-2</v>
       </c>
-      <c r="E157" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A158" s="3">
+      <c r="E158" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A159" s="3">
         <v>46</v>
       </c>
-      <c r="B158" s="2">
+      <c r="B159" s="2">
         <v>24</v>
       </c>
-      <c r="C158" s="3">
+      <c r="C159" s="3">
         <v>4.4526449412279699E-2</v>
       </c>
-      <c r="D158" s="11">
+      <c r="D159" s="11">
         <v>9.3363912416412898E-2</v>
       </c>
-      <c r="E158" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F158" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A159">
+      <c r="E159" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F159" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A160">
         <v>46</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B160" s="1">
         <v>26</v>
       </c>
-      <c r="C159">
+      <c r="C160">
         <v>2.3927451573862699E-2</v>
       </c>
-      <c r="D159" s="12">
+      <c r="D160" s="12">
         <v>9.5650492757272498E-2</v>
       </c>
-      <c r="E159" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A160" s="3">
+      <c r="E160" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A161" s="3">
         <v>47</v>
       </c>
-      <c r="B160" s="3">
+      <c r="B161" s="3">
         <v>28</v>
       </c>
-      <c r="C160" s="3">
+      <c r="C161" s="3">
         <v>1.0025364598100901E-2</v>
       </c>
-      <c r="D160" s="11">
+      <c r="D161" s="11">
         <v>9.7789998658505906E-2</v>
       </c>
-      <c r="E160" s="2">
+      <c r="E161" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F160" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A161">
+      <c r="F161" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A162">
         <v>47</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B162" s="1">
         <v>30</v>
       </c>
-      <c r="C161">
+      <c r="C162">
         <v>3.8033240909878599E-3</v>
       </c>
-      <c r="D161" s="12">
+      <c r="D162" s="12">
         <v>9.9791480572110097E-2</v>
       </c>
-      <c r="E161" s="1">
+      <c r="E162" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A162">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A163">
         <v>48</v>
       </c>
-      <c r="B162" s="1">
+      <c r="B163" s="1">
         <v>22</v>
       </c>
-      <c r="C162">
+      <c r="C163">
         <v>7.6224063203815598E-2</v>
       </c>
-      <c r="D162" s="12">
+      <c r="D163" s="12">
         <v>9.0905259439019295E-2</v>
       </c>
-      <c r="E162" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A163" s="3">
+      <c r="E163" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A164" s="3">
         <v>48</v>
       </c>
-      <c r="B163" s="2">
+      <c r="B164" s="2">
         <v>24</v>
       </c>
-      <c r="C163" s="3">
+      <c r="C164" s="3">
         <v>4.4715112707686903E-2</v>
       </c>
-      <c r="D163" s="11">
+      <c r="D164" s="11">
         <v>9.3350490121472604E-2</v>
       </c>
-      <c r="E163" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F163" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A164">
+      <c r="E164" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F164" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A165">
         <v>48</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B165" s="1">
         <v>26</v>
       </c>
-      <c r="C164">
+      <c r="C165">
         <v>2.4190565368510799E-2</v>
       </c>
-      <c r="D164" s="12">
+      <c r="D165" s="12">
         <v>9.56374813901089E-2</v>
       </c>
-      <c r="E164" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A165" s="3">
+      <c r="E165" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A166" s="3">
         <v>49</v>
       </c>
-      <c r="B165" s="3">
+      <c r="B166" s="3">
         <v>28</v>
       </c>
-      <c r="C165" s="3">
+      <c r="C166" s="3">
         <v>9.5776739104209106E-3</v>
       </c>
-      <c r="D165" s="11">
+      <c r="D166" s="11">
         <v>9.7777665943820202E-2</v>
       </c>
-      <c r="E165" s="2">
+      <c r="E166" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F165" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A166">
+      <c r="F166" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A167">
         <v>49</v>
       </c>
-      <c r="B166" s="1">
+      <c r="B167" s="1">
         <v>30</v>
       </c>
-      <c r="C166">
+      <c r="C167">
         <v>3.7702483227169299E-3</v>
       </c>
-      <c r="D166" s="12">
+      <c r="D167" s="12">
         <v>9.9779187857661003E-2</v>
       </c>
-      <c r="E166" s="1">
+      <c r="E167" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A167">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A168">
         <v>50</v>
       </c>
-      <c r="B167" s="1">
+      <c r="B168" s="1">
         <v>300</v>
       </c>
-      <c r="C167">
-        <v>0</v>
-      </c>
-      <c r="D167" s="12">
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168" s="12">
         <v>6.3402003394675999E-2</v>
       </c>
-      <c r="E167" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A168" s="3">
+      <c r="E168" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A169" s="3">
         <v>50</v>
       </c>
-      <c r="B168" s="2">
+      <c r="B169" s="2">
         <v>387</v>
       </c>
-      <c r="C168" s="3">
-        <v>0</v>
-      </c>
-      <c r="D168" s="11">
+      <c r="C169" s="3">
+        <v>0</v>
+      </c>
+      <c r="D169" s="11">
         <v>6.6013785354650106E-2</v>
       </c>
-      <c r="E168" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F168" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A169">
-        <v>50</v>
-      </c>
-      <c r="B169" s="1">
-        <v>400</v>
-      </c>
-      <c r="C169">
-        <v>0</v>
-      </c>
-      <c r="D169" s="12">
-        <v>6.6362589555679793E-2</v>
-      </c>
-      <c r="E169" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="E169" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F169" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>50</v>
       </c>
       <c r="B170" s="1">
-        <v>455</v>
+        <v>400</v>
       </c>
       <c r="C170">
         <v>0</v>
       </c>
       <c r="D170" s="12">
-        <v>6.7743080399552902E-2</v>
+        <v>6.6362589555679793E-2</v>
       </c>
       <c r="E170" s="1">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>50</v>
       </c>
       <c r="B171" s="1">
+        <v>455</v>
+      </c>
+      <c r="C171">
+        <v>0</v>
+      </c>
+      <c r="D171" s="12">
+        <v>6.7743080399552902E-2</v>
+      </c>
+      <c r="E171" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A172">
+        <v>50</v>
+      </c>
+      <c r="B172" s="1">
         <v>1000</v>
       </c>
-      <c r="C171">
-        <v>0</v>
-      </c>
-      <c r="D171" s="12">
+      <c r="C172">
+        <v>0</v>
+      </c>
+      <c r="D172" s="12">
         <v>7.6668702917551998E-2</v>
       </c>
-      <c r="E171" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A172">
+      <c r="E172" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A173">
         <v>51</v>
       </c>
-      <c r="B172" s="1">
+      <c r="B173" s="1">
         <v>2500</v>
       </c>
-      <c r="C172">
-        <v>0</v>
-      </c>
-      <c r="D172" s="12">
+      <c r="C173">
+        <v>0</v>
+      </c>
+      <c r="D173" s="12">
         <v>8.7400283216006097E-2</v>
       </c>
-      <c r="E172" s="1">
+      <c r="E173" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A173" s="18">
+    <row r="174" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A174" s="18">
         <v>51</v>
       </c>
-      <c r="B173" s="19">
+      <c r="B174" s="19">
         <v>6000</v>
       </c>
-      <c r="C173" s="18">
-        <v>0</v>
-      </c>
-      <c r="D173" s="20">
+      <c r="C174" s="18">
+        <v>0</v>
+      </c>
+      <c r="D174" s="20">
         <v>9.8066863550038699E-2</v>
       </c>
-      <c r="E173" s="19">
+      <c r="E174" s="19">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F173" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A174">
-        <v>51</v>
-      </c>
-      <c r="B174" s="1">
-        <v>6060</v>
-      </c>
-      <c r="C174">
-        <v>0</v>
-      </c>
-      <c r="D174" s="12">
-        <v>9.8189056554440296E-2</v>
-      </c>
-      <c r="E174" s="1">
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F174" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>51</v>
       </c>
       <c r="B175" s="1">
-        <v>10000</v>
+        <v>6060</v>
       </c>
       <c r="C175">
         <v>0</v>
       </c>
       <c r="D175" s="12">
-        <v>0.104293562137796</v>
+        <v>9.8189056554440296E-2</v>
       </c>
       <c r="E175" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176">
+        <v>51</v>
+      </c>
+      <c r="B176" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C176">
+        <v>0</v>
+      </c>
+      <c r="D176" s="12">
+        <v>0.104293562137796</v>
+      </c>
+      <c r="E176" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A177">
         <v>52</v>
       </c>
-      <c r="B176" s="1">
+      <c r="B177" s="1">
         <v>300</v>
       </c>
-      <c r="C176">
-        <v>0</v>
-      </c>
-      <c r="D176" s="12">
+      <c r="C177">
+        <v>0</v>
+      </c>
+      <c r="D177" s="12">
         <v>6.1176881272463401E-2</v>
       </c>
-      <c r="E176" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A177" s="3">
+      <c r="E177" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A178" s="3">
         <v>52</v>
       </c>
-      <c r="B177" s="2">
+      <c r="B178" s="2">
         <v>450</v>
       </c>
-      <c r="C177" s="3">
-        <v>0</v>
-      </c>
-      <c r="D177" s="11">
+      <c r="C178" s="3">
+        <v>0</v>
+      </c>
+      <c r="D178" s="11">
         <v>6.5965078487681003E-2</v>
       </c>
-      <c r="E177" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F177" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A178">
-        <v>52</v>
-      </c>
-      <c r="B178" s="1">
-        <v>455</v>
-      </c>
-      <c r="C178">
-        <v>0</v>
-      </c>
-      <c r="D178" s="12">
-        <v>6.6097731362944404E-2</v>
-      </c>
-      <c r="E178" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="E178" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F178" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>52</v>
       </c>
       <c r="B179" s="1">
+        <v>455</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
+      <c r="D179" s="12">
+        <v>6.6097731362944404E-2</v>
+      </c>
+      <c r="E179" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A180">
+        <v>52</v>
+      </c>
+      <c r="B180" s="1">
         <v>1000</v>
       </c>
-      <c r="C179">
-        <v>0</v>
-      </c>
-      <c r="D179" s="12">
+      <c r="C180">
+        <v>0</v>
+      </c>
+      <c r="D180" s="12">
         <v>7.5813819112299896E-2</v>
       </c>
-      <c r="E179" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A180">
+      <c r="E180" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A181">
         <v>53</v>
       </c>
-      <c r="B180" s="1">
+      <c r="B181" s="1">
         <v>2500</v>
       </c>
-      <c r="C180">
-        <v>0</v>
-      </c>
-      <c r="D180" s="12">
+      <c r="C181">
+        <v>0</v>
+      </c>
+      <c r="D181" s="12">
         <v>8.7024706191877896E-2</v>
       </c>
-      <c r="E180" s="1">
+      <c r="E181" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A181" s="3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A182" s="3">
         <v>53</v>
       </c>
-      <c r="B181" s="2">
+      <c r="B182" s="2">
         <v>6060</v>
       </c>
-      <c r="C181" s="3">
-        <v>0</v>
-      </c>
-      <c r="D181" s="11">
+      <c r="C182" s="3">
+        <v>0</v>
+      </c>
+      <c r="D182" s="11">
         <v>9.8024438005459194E-2</v>
       </c>
-      <c r="E181" s="2">
+      <c r="E182" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F181" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A182">
+      <c r="F182" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A183">
         <v>53</v>
       </c>
-      <c r="B182" s="1">
+      <c r="B183" s="1">
         <v>10000</v>
       </c>
-      <c r="C182">
-        <v>0</v>
-      </c>
-      <c r="D182" s="12">
+      <c r="C183">
+        <v>0</v>
+      </c>
+      <c r="D183" s="12">
         <v>0.104191680713572</v>
       </c>
-      <c r="E182" s="1">
+      <c r="E183" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A183">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A184">
         <v>54</v>
       </c>
-      <c r="B183" s="1">
+      <c r="B184" s="1">
         <v>300</v>
       </c>
-      <c r="C183">
-        <v>0</v>
-      </c>
-      <c r="D183" s="12">
+      <c r="C184">
+        <v>0</v>
+      </c>
+      <c r="D184" s="12">
         <v>6.1102511544927199E-2</v>
       </c>
-      <c r="E183" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A184" s="3">
+      <c r="E184" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A185" s="3">
         <v>54</v>
       </c>
-      <c r="B184" s="2">
+      <c r="B185" s="2">
         <v>455</v>
       </c>
-      <c r="C184" s="3">
-        <v>0</v>
-      </c>
-      <c r="D184" s="11">
+      <c r="C185" s="3">
+        <v>0</v>
+      </c>
+      <c r="D185" s="11">
         <v>6.60498256830475E-2</v>
       </c>
-      <c r="E184" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F184" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A185">
+      <c r="E185" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F185" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A186">
         <v>55</v>
       </c>
-      <c r="B185" s="1">
+      <c r="B186" s="1">
         <v>2500</v>
       </c>
-      <c r="C185">
-        <v>0</v>
-      </c>
-      <c r="D185" s="12">
+      <c r="C186">
+        <v>0</v>
+      </c>
+      <c r="D186" s="12">
         <v>8.7017955666584504E-2</v>
       </c>
-      <c r="E185" s="1">
+      <c r="E186" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A186" s="3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A187" s="3">
         <v>55</v>
       </c>
-      <c r="B186" s="2">
+      <c r="B187" s="2">
         <v>6060</v>
       </c>
-      <c r="C186" s="3">
-        <v>0</v>
-      </c>
-      <c r="D186" s="11">
+      <c r="C187" s="3">
+        <v>0</v>
+      </c>
+      <c r="D187" s="11">
         <v>9.8022066674038899E-2</v>
       </c>
-      <c r="E186" s="2">
+      <c r="E187" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F186" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A187">
+      <c r="F187" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A188">
         <v>55</v>
       </c>
-      <c r="B187" s="1">
+      <c r="B188" s="1">
         <v>10000</v>
       </c>
-      <c r="C187">
-        <v>0</v>
-      </c>
-      <c r="D187" s="12">
+      <c r="C188">
+        <v>0</v>
+      </c>
+      <c r="D188" s="12">
         <v>0.10419035221216499</v>
       </c>
-      <c r="E187" s="1">
+      <c r="E188" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A188">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A189">
         <v>56</v>
       </c>
-      <c r="B188" s="1">
+      <c r="B189" s="1">
         <v>450</v>
       </c>
-      <c r="C188">
-        <v>0</v>
-      </c>
-      <c r="D188" s="12">
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="D189" s="12">
         <v>6.5890773987104106E-2</v>
       </c>
-      <c r="E188" s="15">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A189" s="18">
+      <c r="E189" s="15">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A190" s="18">
         <v>56</v>
       </c>
-      <c r="B189" s="19">
+      <c r="B190" s="19">
         <v>455</v>
       </c>
-      <c r="C189" s="18">
-        <v>0</v>
-      </c>
-      <c r="D189" s="20">
+      <c r="C190" s="18">
+        <v>0</v>
+      </c>
+      <c r="D190" s="20">
         <v>6.60240165647802E-2</v>
       </c>
-      <c r="E189" s="19">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F189" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A190">
+      <c r="E190" s="19">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F190" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A191">
         <v>57</v>
       </c>
-      <c r="B190" s="1">
+      <c r="B191" s="1">
         <v>6000</v>
       </c>
-      <c r="C190">
-        <v>0</v>
-      </c>
-      <c r="D190" s="12">
+      <c r="C191">
+        <v>0</v>
+      </c>
+      <c r="D191" s="12">
         <v>9.7896672921604394E-2</v>
       </c>
-      <c r="E190" s="1">
+      <c r="E191" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A191" s="3">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A192" s="3">
         <v>57</v>
       </c>
-      <c r="B191" s="2">
+      <c r="B192" s="2">
         <v>6060</v>
       </c>
-      <c r="C191" s="3">
-        <v>0</v>
-      </c>
-      <c r="D191" s="11">
+      <c r="C192" s="3">
+        <v>0</v>
+      </c>
+      <c r="D192" s="11">
         <v>9.8020389223630294E-2</v>
       </c>
-      <c r="E191" s="2">
+      <c r="E192" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F191" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A192">
+      <c r="F192" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A193">
         <v>58</v>
       </c>
-      <c r="B192" s="1">
+      <c r="B193" s="1">
         <v>430</v>
       </c>
-      <c r="C192">
-        <v>0</v>
-      </c>
-      <c r="D192" s="12">
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193" s="12">
         <v>6.5369257078097903E-2</v>
       </c>
-      <c r="E192" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A193" s="3">
+      <c r="E193" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A194" s="3">
         <v>58</v>
       </c>
-      <c r="B193" s="2">
+      <c r="B194" s="2">
         <v>455</v>
       </c>
-      <c r="C193" s="3">
-        <v>0</v>
-      </c>
-      <c r="D193" s="11">
+      <c r="C194" s="3">
+        <v>0</v>
+      </c>
+      <c r="D194" s="11">
         <v>6.60498256830475E-2</v>
       </c>
-      <c r="E193" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F193" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A194">
+      <c r="E194" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F194" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A195">
         <v>59</v>
       </c>
-      <c r="B194" s="1">
+      <c r="B195" s="1">
         <v>6000</v>
       </c>
-      <c r="C194">
-        <v>0</v>
-      </c>
-      <c r="D194" s="12">
+      <c r="C195">
+        <v>0</v>
+      </c>
+      <c r="D195" s="12">
         <v>9.7898414715878707E-2</v>
       </c>
-      <c r="E194" s="1">
+      <c r="E195" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A195" s="3">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A196" s="3">
         <v>59</v>
       </c>
-      <c r="B195" s="2">
+      <c r="B196" s="2">
         <v>6060</v>
       </c>
-      <c r="C195" s="3">
-        <v>0</v>
-      </c>
-      <c r="D195" s="11">
+      <c r="C196" s="3">
+        <v>0</v>
+      </c>
+      <c r="D196" s="11">
         <v>9.8022066674038899E-2</v>
       </c>
-      <c r="E195" s="2">
+      <c r="E196" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F195" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A196">
+      <c r="F196" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A197">
         <v>60</v>
       </c>
-      <c r="B196" s="1">
+      <c r="B197" s="1">
         <v>430</v>
       </c>
-      <c r="C196">
-        <v>0</v>
-      </c>
-      <c r="D196" s="12">
+      <c r="C197">
+        <v>0</v>
+      </c>
+      <c r="D197" s="12">
         <v>6.5420029806049898E-2</v>
       </c>
-      <c r="E196" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A197" s="3">
+      <c r="E197" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A198" s="3">
         <v>60</v>
       </c>
-      <c r="B197" s="2">
+      <c r="B198" s="2">
         <v>455</v>
       </c>
-      <c r="C197" s="3">
-        <v>0</v>
-      </c>
-      <c r="D197" s="11">
+      <c r="C198" s="3">
+        <v>0</v>
+      </c>
+      <c r="D198" s="11">
         <v>6.6097731362944404E-2</v>
       </c>
-      <c r="E197" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F197" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A198">
+      <c r="E198" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F198" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A199">
         <v>61</v>
       </c>
-      <c r="B198" s="1">
+      <c r="B199" s="1">
         <v>6000</v>
       </c>
-      <c r="C198">
-        <v>0</v>
-      </c>
-      <c r="D198" s="12">
+      <c r="C199">
+        <v>0</v>
+      </c>
+      <c r="D199" s="12">
         <v>9.7900886871799903E-2</v>
       </c>
-      <c r="E198" s="1">
+      <c r="E199" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A199" s="3">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A200" s="3">
         <v>61</v>
       </c>
-      <c r="B199" s="2">
+      <c r="B200" s="2">
         <v>6060</v>
       </c>
-      <c r="C199" s="3">
-        <v>0</v>
-      </c>
-      <c r="D199" s="11">
+      <c r="C200" s="3">
+        <v>0</v>
+      </c>
+      <c r="D200" s="11">
         <v>9.8024438005459194E-2</v>
       </c>
-      <c r="E199" s="2">
+      <c r="E200" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F199" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A200">
+      <c r="F200" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A201">
         <v>62</v>
       </c>
-      <c r="B200" s="1">
+      <c r="B201" s="1">
         <v>440</v>
       </c>
-      <c r="C200">
-        <v>0</v>
-      </c>
-      <c r="D200" s="12">
+      <c r="C201">
+        <v>0</v>
+      </c>
+      <c r="D201" s="12">
         <v>6.5618982861038094E-2</v>
       </c>
-      <c r="E200" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A201" s="3">
+      <c r="E201" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A202" s="3">
         <v>62</v>
       </c>
-      <c r="B201" s="2">
+      <c r="B202" s="2">
         <v>455</v>
       </c>
-      <c r="C201" s="3">
-        <v>0</v>
-      </c>
-      <c r="D201" s="11">
+      <c r="C202" s="3">
+        <v>0</v>
+      </c>
+      <c r="D202" s="11">
         <v>6.6023657650045295E-2</v>
       </c>
-      <c r="E201" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F201" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A202">
+      <c r="E202" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F202" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A203">
         <v>63</v>
       </c>
-      <c r="B202" s="1">
+      <c r="B203" s="1">
         <v>6000</v>
       </c>
-      <c r="C202">
-        <v>0</v>
-      </c>
-      <c r="D202" s="12">
+      <c r="C203">
+        <v>0</v>
+      </c>
+      <c r="D203" s="12">
         <v>9.7896668269247006E-2</v>
       </c>
-      <c r="E202" s="1">
+      <c r="E203" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A203" s="3">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A204" s="3">
         <v>63</v>
       </c>
-      <c r="B203" s="2">
+      <c r="B204" s="2">
         <v>6060</v>
       </c>
-      <c r="C203" s="3">
-        <v>0</v>
-      </c>
-      <c r="D203" s="11">
+      <c r="C204" s="3">
+        <v>0</v>
+      </c>
+      <c r="D204" s="11">
         <v>9.8020384167614896E-2</v>
       </c>
-      <c r="E203" s="2">
+      <c r="E204" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F203" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A204">
+      <c r="F204" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A205">
         <v>64</v>
       </c>
-      <c r="B204" s="1">
+      <c r="B205" s="1">
         <v>440</v>
       </c>
-      <c r="C204">
-        <v>0</v>
-      </c>
-      <c r="D204" s="12">
+      <c r="C205">
+        <v>0</v>
+      </c>
+      <c r="D205" s="12">
         <v>6.5619334125610995E-2</v>
       </c>
-      <c r="E204" s="1">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A205" s="3">
+      <c r="E205" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A206" s="3">
         <v>64</v>
       </c>
-      <c r="B205" s="2">
+      <c r="B206" s="2">
         <v>455</v>
       </c>
-      <c r="C205" s="3">
-        <v>0</v>
-      </c>
-      <c r="D205" s="11">
+      <c r="C206" s="3">
+        <v>0</v>
+      </c>
+      <c r="D206" s="11">
         <v>6.60240165647802E-2</v>
       </c>
-      <c r="E205" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F205" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A206">
+      <c r="E206" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F206" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A207">
         <v>65</v>
       </c>
-      <c r="B206" s="1">
+      <c r="B207" s="1">
         <v>6000</v>
       </c>
-      <c r="C206">
-        <v>0</v>
-      </c>
-      <c r="D206" s="12">
+      <c r="C207">
+        <v>0</v>
+      </c>
+      <c r="D207" s="12">
         <v>9.7896672921604394E-2</v>
       </c>
-      <c r="E206" s="1">
+      <c r="E207" s="1">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A207" s="3">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A208" s="3">
         <v>65</v>
       </c>
-      <c r="B207" s="2">
+      <c r="B208" s="2">
         <v>6060</v>
       </c>
-      <c r="C207" s="3">
-        <v>0</v>
-      </c>
-      <c r="D207" s="11">
+      <c r="C208" s="3">
+        <v>0</v>
+      </c>
+      <c r="D208" s="11">
         <v>9.8020389223630294E-2</v>
       </c>
-      <c r="E207" s="2">
+      <c r="E208" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F207" s="3">
-        <v>1</v>
+      <c r="F208" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A209">
+        <v>66</v>
+      </c>
+      <c r="B209" s="1">
+        <v>200</v>
+      </c>
+      <c r="E209" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A210">
+        <v>66</v>
+      </c>
+      <c r="B210" s="1">
+        <v>400</v>
+      </c>
+      <c r="E210" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A211">
+        <v>66</v>
+      </c>
+      <c r="B211" s="1">
+        <v>600</v>
+      </c>
+      <c r="E211" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>66</v>
+      </c>
+      <c r="B212" s="1">
+        <v>900</v>
+      </c>
+      <c r="E212" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A213">
+        <v>66</v>
+      </c>
+      <c r="B213" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E213" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>66</v>
+      </c>
+      <c r="B214" s="1">
+        <v>1600</v>
+      </c>
+      <c r="E214" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A215">
+        <v>66</v>
+      </c>
+      <c r="B215" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E215" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A216">
+        <v>66</v>
+      </c>
+      <c r="B216" s="1">
+        <v>2500</v>
+      </c>
+      <c r="E216" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A217">
+        <v>66</v>
+      </c>
+      <c r="B217" s="1">
+        <v>3000</v>
+      </c>
+      <c r="E217" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A218">
+        <v>66</v>
+      </c>
+      <c r="B218" s="1">
+        <v>4000</v>
+      </c>
+      <c r="E218" s="1">
+        <v>6.6000000000000003E-2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F207">
-    <filterColumn colId="5">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F208"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>